<commit_message>
updated Textile files for obj104, pic200, pic201
</commit_message>
<xml_diff>
--- a/externals/Eve_web_catalog.xlsx
+++ b/externals/Eve_web_catalog.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7240" yWindow="2760" windowWidth="20020" windowHeight="13380" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="3020" yWindow="640" windowWidth="29240" windowHeight="16680" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" r:id="rId1"/>
     <sheet name="Images" sheetId="2" r:id="rId2"/>
     <sheet name="Albums" sheetId="3" r:id="rId3"/>
+    <sheet name="Types and Tags" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="499">
   <si>
     <t>000025-01</t>
   </si>
@@ -1478,9 +1479,6 @@
     <t>pic000204</t>
   </si>
   <si>
-    <t>alb000203</t>
-  </si>
-  <si>
     <t>2015-07-26-pic000203</t>
   </si>
   <si>
@@ -1491,13 +1489,43 @@
   </si>
   <si>
     <t>alb000103</t>
+  </si>
+  <si>
+    <t>pic000205</t>
+  </si>
+  <si>
+    <t>pic000206</t>
+  </si>
+  <si>
+    <t>alb000104</t>
+  </si>
+  <si>
+    <t>artist's book</t>
+  </si>
+  <si>
+    <t>TYPES</t>
+  </si>
+  <si>
+    <t>TAGS</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000102-01.textile</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000205</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000206</t>
+  </si>
+  <si>
+    <t>PHOTO NUMBER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1534,6 +1562,20 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1625,7 +1667,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1633,6 +1675,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2032,8 +2075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I73"/>
   <sheetViews>
-    <sheetView topLeftCell="C32" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView topLeftCell="A13" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3002,7 +3045,7 @@
         <v>467</v>
       </c>
       <c r="B40" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C40" t="s">
         <v>3</v>
@@ -3020,13 +3063,34 @@
         <v>484</v>
       </c>
       <c r="H40" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="3" t="s">
         <v>468</v>
       </c>
+      <c r="B41" t="s">
+        <v>495</v>
+      </c>
+      <c r="C41" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" t="s">
+        <v>399</v>
+      </c>
+      <c r="F41" t="s">
+        <v>420</v>
+      </c>
+      <c r="G41" t="s">
+        <v>490</v>
+      </c>
+      <c r="H41" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="4" t="s">
@@ -3285,8 +3349,9 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3297,25 +3362,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I145"/>
+  <dimension ref="A2:J147"/>
   <sheetViews>
-    <sheetView topLeftCell="A126" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H145" sqref="H145"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29.1640625" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" customWidth="1"/>
-    <col min="3" max="3" width="3.1640625" customWidth="1"/>
-    <col min="4" max="4" width="2.83203125" customWidth="1"/>
-    <col min="5" max="5" width="2.1640625" customWidth="1"/>
-    <col min="6" max="6" width="2.83203125" customWidth="1"/>
-    <col min="7" max="7" width="2.5" customWidth="1"/>
-    <col min="8" max="8" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="3.1640625" customWidth="1"/>
+    <col min="5" max="5" width="2.83203125" customWidth="1"/>
+    <col min="6" max="6" width="2.1640625" customWidth="1"/>
+    <col min="7" max="7" width="2.83203125" customWidth="1"/>
+    <col min="8" max="8" width="2.5" customWidth="1"/>
+    <col min="9" max="9" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>151</v>
       </c>
@@ -3323,47 +3389,50 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
+        <v>498</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>144</v>
       </c>
       <c r="B3" t="s">
         <v>145</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>146</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>98</v>
       </c>
@@ -3375,1548 +3444,1579 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="C6" s="1"/>
+      <c r="I6" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>153</v>
       </c>
       <c r="B8" t="s">
         <v>152</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>156</v>
       </c>
       <c r="B9" t="s">
         <v>155</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>158</v>
       </c>
       <c r="B10" t="s">
         <v>157</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>159</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>162</v>
       </c>
       <c r="B12" t="s">
         <v>161</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>25</v>
       </c>
       <c r="B13" t="s">
         <v>163</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>165</v>
       </c>
       <c r="B14" t="s">
         <v>164</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>41</v>
       </c>
       <c r="B15" t="s">
         <v>166</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>46</v>
       </c>
       <c r="B16" t="s">
         <v>168</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>171</v>
       </c>
       <c r="B17" t="s">
         <v>170</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>174</v>
       </c>
       <c r="B18" t="s">
         <v>173</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>177</v>
       </c>
       <c r="B19" t="s">
         <v>176</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>179</v>
       </c>
       <c r="B20" t="s">
         <v>178</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>182</v>
       </c>
       <c r="B21" t="s">
         <v>181</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>184</v>
       </c>
       <c r="B22" t="s">
         <v>183</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>186</v>
       </c>
       <c r="B23" t="s">
         <v>185</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>188</v>
       </c>
       <c r="B24" t="s">
         <v>187</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>190</v>
       </c>
       <c r="B25" t="s">
         <v>189</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>192</v>
       </c>
       <c r="B26" t="s">
         <v>191</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>194</v>
       </c>
       <c r="B27" t="s">
         <v>193</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>196</v>
       </c>
       <c r="B28" t="s">
         <v>195</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>198</v>
       </c>
       <c r="B29" t="s">
         <v>197</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
         <v>200</v>
       </c>
       <c r="B30" t="s">
         <v>199</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>202</v>
       </c>
       <c r="B31" t="s">
         <v>201</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>59</v>
       </c>
       <c r="B32" t="s">
         <v>203</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>52</v>
       </c>
       <c r="B33" t="s">
         <v>205</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>207</v>
       </c>
       <c r="B34" t="s">
         <v>206</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>56</v>
       </c>
       <c r="B35" t="s">
         <v>209</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>212</v>
       </c>
       <c r="B36" t="s">
         <v>211</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>214</v>
       </c>
       <c r="B37" t="s">
         <v>213</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>63</v>
       </c>
       <c r="B38" t="s">
         <v>61</v>
       </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>216</v>
       </c>
       <c r="B39" t="s">
         <v>215</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
         <v>66</v>
       </c>
       <c r="B40" t="s">
         <v>64</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>218</v>
       </c>
       <c r="B41" t="s">
         <v>217</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>220</v>
       </c>
       <c r="B42" t="s">
         <v>219</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>70</v>
       </c>
       <c r="B43" t="s">
         <v>221</v>
       </c>
-      <c r="H43" t="s">
+      <c r="I43" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>29</v>
       </c>
       <c r="B44" t="s">
         <v>222</v>
       </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>37</v>
       </c>
       <c r="B45" t="s">
         <v>223</v>
       </c>
-      <c r="H45" t="s">
+      <c r="I45" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>73</v>
       </c>
       <c r="B46" t="s">
         <v>224</v>
       </c>
-      <c r="H46" t="s">
+      <c r="I46" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>226</v>
       </c>
       <c r="B47" t="s">
         <v>225</v>
       </c>
-      <c r="H47" t="s">
+      <c r="I47" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>228</v>
       </c>
       <c r="B48" t="s">
         <v>227</v>
       </c>
-      <c r="H48" t="s">
+      <c r="I48" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>230</v>
       </c>
       <c r="B49" t="s">
         <v>229</v>
       </c>
-      <c r="H49" t="s">
+      <c r="I49" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>78</v>
       </c>
       <c r="B50" t="s">
         <v>75</v>
       </c>
-      <c r="H50" t="s">
+      <c r="I50" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>21</v>
       </c>
       <c r="B51" t="s">
         <v>231</v>
       </c>
-      <c r="H51" t="s">
+      <c r="I51" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>81</v>
       </c>
       <c r="B52" t="s">
         <v>232</v>
       </c>
-      <c r="H52" t="s">
+      <c r="I52" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>234</v>
       </c>
       <c r="B53" t="s">
         <v>233</v>
       </c>
-      <c r="H53" t="s">
+      <c r="I53" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>236</v>
       </c>
       <c r="B54" t="s">
         <v>235</v>
       </c>
-      <c r="H54" t="s">
+      <c r="I54" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>237</v>
       </c>
       <c r="B55" t="s">
         <v>83</v>
       </c>
-      <c r="H55" t="s">
+      <c r="I55" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
         <v>89</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="H56" t="s">
+      <c r="C56" s="2"/>
+      <c r="I56" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:9">
       <c r="A57" t="s">
         <v>241</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="H57" t="s">
+      <c r="C57" s="2"/>
+      <c r="I57" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:9">
       <c r="A58" t="s">
         <v>243</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="H58" t="s">
+      <c r="C58" s="2"/>
+      <c r="I58" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
         <v>238</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="H59" t="s">
+      <c r="C59" s="2"/>
+      <c r="I59" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:9">
       <c r="A60" t="s">
         <v>246</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="H60" t="s">
+      <c r="C60" s="2"/>
+      <c r="I60" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:9">
       <c r="A61" t="s">
         <v>248</v>
       </c>
       <c r="B61" t="s">
         <v>247</v>
       </c>
-      <c r="H61" t="s">
+      <c r="I61" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:9">
       <c r="A62" t="s">
         <v>250</v>
       </c>
       <c r="B62" t="s">
         <v>249</v>
       </c>
-      <c r="H62" t="s">
+      <c r="I62" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:9">
       <c r="A63" t="s">
         <v>252</v>
       </c>
       <c r="B63" t="s">
         <v>251</v>
       </c>
-      <c r="H63" t="s">
+      <c r="I63" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:9">
       <c r="A64" t="s">
         <v>254</v>
       </c>
       <c r="B64" t="s">
         <v>253</v>
       </c>
-      <c r="H64" t="s">
+      <c r="I64" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:9">
       <c r="A65" t="s">
         <v>256</v>
       </c>
       <c r="B65" t="s">
         <v>255</v>
       </c>
-      <c r="H65" t="s">
+      <c r="I65" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:9">
       <c r="A66" t="s">
         <v>258</v>
       </c>
       <c r="B66" t="s">
         <v>257</v>
       </c>
-      <c r="H66" t="s">
+      <c r="I66" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:9">
       <c r="A67" t="s">
         <v>260</v>
       </c>
       <c r="B67" t="s">
         <v>259</v>
       </c>
-      <c r="H67" t="s">
+      <c r="I67" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:9">
       <c r="A68" t="s">
         <v>98</v>
       </c>
       <c r="B68" t="s">
         <v>95</v>
       </c>
-      <c r="H68" t="s">
+      <c r="I68" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:9">
       <c r="A69" t="s">
         <v>102</v>
       </c>
       <c r="B69" t="s">
         <v>261</v>
       </c>
-      <c r="H69" t="s">
+      <c r="I69" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:9">
       <c r="A70" t="s">
         <v>262</v>
       </c>
       <c r="B70" t="s">
         <v>99</v>
       </c>
-      <c r="H70" t="s">
+      <c r="I70" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:9">
       <c r="A71" t="s">
         <v>106</v>
       </c>
       <c r="B71" t="s">
         <v>103</v>
       </c>
-      <c r="H71" t="s">
+      <c r="I71" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:9">
       <c r="A72" t="s">
         <v>265</v>
       </c>
       <c r="B72" t="s">
         <v>264</v>
       </c>
-      <c r="H72" t="s">
+      <c r="I72" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:9">
       <c r="A73" t="s">
         <v>268</v>
       </c>
       <c r="B73" t="s">
         <v>267</v>
       </c>
-      <c r="H73" t="s">
+      <c r="I73" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:9">
       <c r="A74" t="s">
         <v>113</v>
       </c>
       <c r="B74" t="s">
         <v>270</v>
       </c>
-      <c r="H74" t="s">
+      <c r="I74" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:9">
       <c r="A75" t="s">
         <v>272</v>
       </c>
       <c r="B75" t="s">
         <v>271</v>
       </c>
-      <c r="H75" t="s">
+      <c r="I75" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:9">
       <c r="A76" t="s">
         <v>274</v>
       </c>
       <c r="B76" t="s">
         <v>273</v>
       </c>
-      <c r="H76" t="s">
+      <c r="I76" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:9">
       <c r="A77" t="s">
         <v>276</v>
       </c>
       <c r="B77" t="s">
         <v>275</v>
       </c>
-      <c r="H77" t="s">
+      <c r="I77" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:9">
       <c r="A78" t="s">
         <v>278</v>
       </c>
       <c r="B78" t="s">
         <v>277</v>
       </c>
-      <c r="H78" t="s">
+      <c r="I78" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:9">
       <c r="A79" t="s">
         <v>280</v>
       </c>
       <c r="B79" t="s">
         <v>279</v>
       </c>
-      <c r="H79" t="s">
+      <c r="I79" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:9">
       <c r="A80" t="s">
         <v>282</v>
       </c>
       <c r="B80" t="s">
         <v>281</v>
       </c>
-      <c r="H80" t="s">
+      <c r="I80" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:9">
       <c r="A81" t="s">
         <v>284</v>
       </c>
       <c r="B81" t="s">
         <v>283</v>
       </c>
-      <c r="H81" t="s">
+      <c r="I81" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:9">
       <c r="A82" t="s">
         <v>286</v>
       </c>
       <c r="B82" t="s">
         <v>285</v>
       </c>
-      <c r="H82" t="s">
+      <c r="I82" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:9">
       <c r="A83" t="s">
         <v>288</v>
       </c>
       <c r="B83" t="s">
         <v>287</v>
       </c>
-      <c r="H83" t="s">
+      <c r="I83" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:9">
       <c r="A84" t="s">
         <v>290</v>
       </c>
       <c r="B84" t="s">
         <v>289</v>
       </c>
-      <c r="H84" t="s">
+      <c r="I84" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:9">
       <c r="A85" t="s">
         <v>292</v>
       </c>
       <c r="B85" t="s">
         <v>291</v>
       </c>
-      <c r="H85" t="s">
+      <c r="I85" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:9">
       <c r="A86" t="s">
         <v>294</v>
       </c>
       <c r="B86" t="s">
         <v>293</v>
       </c>
-      <c r="H86" t="s">
+      <c r="I86" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:9">
       <c r="A87" t="s">
         <v>296</v>
       </c>
       <c r="B87" t="s">
         <v>295</v>
       </c>
-      <c r="H87" t="s">
+      <c r="I87" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:9">
       <c r="A88" t="s">
         <v>118</v>
       </c>
       <c r="B88" t="s">
         <v>115</v>
       </c>
-      <c r="H88" t="s">
+      <c r="I88" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:9">
       <c r="A89" t="s">
         <v>122</v>
       </c>
       <c r="B89" t="s">
         <v>119</v>
       </c>
-      <c r="H89" t="s">
+      <c r="I89" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:9">
       <c r="A90" t="s">
         <v>299</v>
       </c>
       <c r="B90" t="s">
         <v>123</v>
       </c>
-      <c r="H90" t="s">
+      <c r="I90" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:9">
       <c r="A91" t="s">
         <v>302</v>
       </c>
       <c r="B91" t="s">
         <v>301</v>
       </c>
-      <c r="H91" t="s">
+      <c r="I91" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:9">
       <c r="A92" t="s">
         <v>305</v>
       </c>
       <c r="B92" t="s">
         <v>304</v>
       </c>
-      <c r="H92" t="s">
+      <c r="I92" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:9">
       <c r="A93" t="s">
         <v>17</v>
       </c>
       <c r="B93" t="s">
         <v>306</v>
       </c>
-      <c r="H93" t="s">
+      <c r="I93" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:9">
       <c r="A94" t="s">
         <v>128</v>
       </c>
       <c r="B94" t="s">
         <v>126</v>
       </c>
-      <c r="H94" t="s">
+      <c r="I94" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:9">
       <c r="A95" t="s">
         <v>308</v>
       </c>
       <c r="B95" t="s">
         <v>307</v>
       </c>
-      <c r="H95" t="s">
+      <c r="I95" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:9">
       <c r="A96" t="s">
         <v>132</v>
       </c>
       <c r="B96" t="s">
         <v>129</v>
       </c>
-      <c r="H96" t="s">
+      <c r="I96" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:9">
       <c r="A97" t="s">
         <v>311</v>
       </c>
       <c r="B97" t="s">
         <v>310</v>
       </c>
-      <c r="H97" t="s">
+      <c r="I97" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:9">
       <c r="A98" t="s">
         <v>313</v>
       </c>
       <c r="B98" t="s">
         <v>312</v>
       </c>
-      <c r="H98" t="s">
+      <c r="I98" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:9">
       <c r="A99" t="s">
         <v>316</v>
       </c>
       <c r="B99" t="s">
         <v>315</v>
       </c>
-      <c r="H99" t="s">
+      <c r="I99" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:9">
       <c r="A100" t="s">
         <v>317</v>
       </c>
       <c r="B100" t="s">
         <v>133</v>
       </c>
-      <c r="H100" t="s">
+      <c r="I100" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:9">
       <c r="A101" t="s">
         <v>139</v>
       </c>
       <c r="B101" t="s">
         <v>136</v>
       </c>
-      <c r="H101" t="s">
+      <c r="I101" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:9">
       <c r="A102" t="s">
         <v>109</v>
       </c>
       <c r="B102" t="s">
         <v>319</v>
       </c>
-      <c r="H102" t="s">
+      <c r="I102" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:9">
       <c r="A103" t="s">
         <v>321</v>
       </c>
       <c r="B103" t="s">
         <v>320</v>
       </c>
-      <c r="H103" t="s">
+      <c r="I103" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:9">
       <c r="A104" t="s">
         <v>323</v>
       </c>
       <c r="B104" t="s">
         <v>322</v>
       </c>
-      <c r="H104" t="s">
+      <c r="I104" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:9">
       <c r="A105" t="s">
         <v>325</v>
       </c>
       <c r="B105" t="s">
         <v>324</v>
       </c>
-      <c r="H105" t="s">
+      <c r="I105" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:9">
       <c r="A106" t="s">
         <v>327</v>
       </c>
       <c r="B106" t="s">
         <v>326</v>
       </c>
-      <c r="H106" t="s">
+      <c r="I106" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:9">
       <c r="A107" t="s">
         <v>329</v>
       </c>
       <c r="B107" t="s">
         <v>328</v>
       </c>
-      <c r="H107" t="s">
+      <c r="I107" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:9">
       <c r="A108" t="s">
         <v>331</v>
       </c>
       <c r="B108" t="s">
         <v>330</v>
       </c>
-      <c r="H108" t="s">
+      <c r="I108" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:9">
       <c r="A109" t="s">
         <v>333</v>
       </c>
       <c r="B109" t="s">
         <v>332</v>
       </c>
-      <c r="H109" t="s">
+      <c r="I109" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:9">
       <c r="A110" t="s">
         <v>335</v>
       </c>
       <c r="B110" t="s">
         <v>334</v>
       </c>
-      <c r="H110" t="s">
+      <c r="I110" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:9">
       <c r="A111" t="s">
         <v>337</v>
       </c>
       <c r="B111" t="s">
         <v>336</v>
       </c>
-      <c r="H111" t="s">
+      <c r="I111" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:9">
       <c r="A112" t="s">
         <v>339</v>
       </c>
       <c r="B112" t="s">
         <v>338</v>
       </c>
-      <c r="H112" t="s">
+      <c r="I112" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:9">
       <c r="A113" t="s">
         <v>341</v>
       </c>
       <c r="B113" t="s">
         <v>340</v>
       </c>
-      <c r="H113" t="s">
+      <c r="I113" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:9">
       <c r="A114" t="s">
         <v>343</v>
       </c>
       <c r="B114" t="s">
         <v>342</v>
       </c>
-      <c r="H114" t="s">
+      <c r="I114" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:9">
       <c r="A115" t="s">
         <v>142</v>
       </c>
       <c r="B115" t="s">
         <v>344</v>
       </c>
-      <c r="H115" t="s">
+      <c r="I115" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:9">
       <c r="A116" t="s">
         <v>346</v>
       </c>
       <c r="B116" t="s">
         <v>345</v>
       </c>
-      <c r="H116" t="s">
+      <c r="I116" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:9">
       <c r="A117" t="s">
         <v>348</v>
       </c>
       <c r="B117" t="s">
         <v>347</v>
       </c>
-      <c r="H117" t="s">
+      <c r="I117" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:9">
       <c r="A118" t="s">
         <v>350</v>
       </c>
       <c r="B118" t="s">
         <v>349</v>
       </c>
-      <c r="H118" t="s">
+      <c r="I118" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:9">
       <c r="A119" t="s">
         <v>352</v>
       </c>
       <c r="B119" t="s">
         <v>351</v>
       </c>
-      <c r="H119" t="s">
+      <c r="I119" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:9">
       <c r="A120" t="s">
         <v>354</v>
       </c>
       <c r="B120" t="s">
         <v>353</v>
       </c>
-      <c r="H120" t="s">
+      <c r="I120" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:9">
       <c r="A121" t="s">
         <v>356</v>
       </c>
       <c r="B121" t="s">
         <v>355</v>
       </c>
-      <c r="H121" t="s">
+      <c r="I121" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:9">
       <c r="A122" t="s">
         <v>358</v>
       </c>
       <c r="B122" t="s">
         <v>357</v>
       </c>
-      <c r="H122" t="s">
+      <c r="I122" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:9">
       <c r="A123" t="s">
         <v>360</v>
       </c>
       <c r="B123" t="s">
         <v>359</v>
       </c>
-      <c r="H123" t="s">
+      <c r="I123" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:9">
       <c r="A124" t="s">
         <v>362</v>
       </c>
       <c r="B124" t="s">
         <v>361</v>
       </c>
-      <c r="H124" t="s">
+      <c r="I124" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:9">
       <c r="A125" t="s">
         <v>364</v>
       </c>
       <c r="B125" t="s">
         <v>363</v>
       </c>
-      <c r="H125" t="s">
+      <c r="I125" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:9">
       <c r="A126" t="s">
         <v>366</v>
       </c>
       <c r="B126" t="s">
         <v>365</v>
       </c>
-      <c r="H126" t="s">
+      <c r="I126" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:9">
       <c r="A127" t="s">
         <v>368</v>
       </c>
       <c r="B127" t="s">
         <v>367</v>
       </c>
-      <c r="H127" t="s">
+      <c r="I127" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:9">
       <c r="A128" t="s">
         <v>370</v>
       </c>
       <c r="B128" t="s">
         <v>369</v>
       </c>
-      <c r="H128" t="s">
+      <c r="I128" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:9">
       <c r="A129" t="s">
         <v>372</v>
       </c>
       <c r="B129" t="s">
         <v>371</v>
       </c>
-      <c r="H129" t="s">
+      <c r="I129" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:9">
       <c r="A130" t="s">
         <v>374</v>
       </c>
       <c r="B130" t="s">
         <v>373</v>
       </c>
-      <c r="H130" t="s">
+      <c r="I130" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:9">
       <c r="A131" t="s">
         <v>376</v>
       </c>
       <c r="B131" t="s">
         <v>375</v>
       </c>
-      <c r="H131" t="s">
+      <c r="I131" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:9">
       <c r="A132" t="s">
         <v>378</v>
       </c>
       <c r="B132" t="s">
         <v>377</v>
       </c>
-      <c r="H132" t="s">
+      <c r="I132" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:9">
       <c r="A133" t="s">
         <v>380</v>
       </c>
       <c r="B133" t="s">
         <v>379</v>
       </c>
-      <c r="H133" t="s">
+      <c r="I133" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:9">
       <c r="A134" t="s">
         <v>382</v>
       </c>
       <c r="B134" t="s">
         <v>381</v>
       </c>
-      <c r="H134" t="s">
+      <c r="I134" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:9">
       <c r="A135" t="s">
         <v>384</v>
       </c>
       <c r="B135" t="s">
         <v>383</v>
       </c>
-      <c r="H135" t="s">
+      <c r="I135" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:9">
       <c r="A136" t="s">
         <v>386</v>
       </c>
       <c r="B136" t="s">
         <v>385</v>
       </c>
-      <c r="H136" t="s">
+      <c r="I136" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:9">
       <c r="A137" t="s">
         <v>388</v>
       </c>
       <c r="B137" t="s">
         <v>387</v>
       </c>
-      <c r="H137" t="s">
+      <c r="I137" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:9">
       <c r="A138" t="s">
         <v>390</v>
       </c>
       <c r="B138" t="s">
         <v>389</v>
       </c>
-      <c r="H138" t="s">
+      <c r="I138" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:9">
       <c r="A139" t="s">
         <v>392</v>
       </c>
       <c r="B139" t="s">
         <v>391</v>
       </c>
-      <c r="H139" t="s">
+      <c r="I139" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:9">
       <c r="A140" t="s">
         <v>394</v>
       </c>
       <c r="B140" t="s">
         <v>393</v>
       </c>
-      <c r="H140" t="s">
+      <c r="I140" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:9">
       <c r="A141" t="s">
         <v>428</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="H141" t="s">
+      <c r="C141" s="3"/>
+      <c r="I141" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:9">
       <c r="A142" t="s">
         <v>434</v>
       </c>
       <c r="B142" t="s">
         <v>431</v>
       </c>
-      <c r="H142" t="s">
+      <c r="I142" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:9">
       <c r="A143" t="s">
         <v>430</v>
       </c>
       <c r="B143" t="s">
         <v>429</v>
       </c>
-      <c r="H143" t="s">
+      <c r="I143" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:9">
       <c r="A144" t="s">
         <v>483</v>
       </c>
       <c r="B144" t="s">
-        <v>486</v>
-      </c>
-      <c r="H144" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="145" spans="1:8">
+      <c r="I144" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9">
       <c r="A145" t="s">
         <v>484</v>
       </c>
       <c r="B145" t="s">
-        <v>487</v>
-      </c>
-      <c r="H145" t="s">
-        <v>485</v>
+        <v>486</v>
+      </c>
+      <c r="I145" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9">
+      <c r="A146" t="s">
+        <v>489</v>
+      </c>
+      <c r="B146" t="s">
+        <v>496</v>
+      </c>
+      <c r="I146" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9">
+      <c r="A147" t="s">
+        <v>490</v>
+      </c>
+      <c r="B147" t="s">
+        <v>497</v>
+      </c>
+      <c r="I147" t="s">
+        <v>491</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4927,10 +5027,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:B10"/>
+  <dimension ref="B4:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4957,12 +5057,54 @@
     </row>
     <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>489</v>
+        <v>488</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" t="s">
+        <v>491</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="28.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4">
+      <c r="B2" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" t="s">
+        <v>492</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
updated recent Textile files
</commit_message>
<xml_diff>
--- a/externals/Eve_web_catalog.xlsx
+++ b/externals/Eve_web_catalog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="40" windowWidth="17260" windowHeight="12860" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="540" yWindow="60" windowWidth="24040" windowHeight="11420" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="509">
   <si>
     <t>000025-01</t>
   </si>
@@ -1540,6 +1540,15 @@
   </si>
   <si>
     <t>S 11-0043</t>
+  </si>
+  <si>
+    <t>pic000207</t>
+  </si>
+  <si>
+    <t>2015-01-31-pic000207.textile</t>
+  </si>
+  <si>
+    <t>S-40-0048</t>
   </si>
 </sst>
 </file>
@@ -2096,8 +2105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I73"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView topLeftCell="A33" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3383,10 +3392,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J147"/>
+  <dimension ref="A2:J148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C146" sqref="C146"/>
+    <sheetView tabSelected="1" topLeftCell="A137" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I149" sqref="I149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5052,6 +5061,20 @@
       </c>
       <c r="I147" t="s">
         <v>491</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9">
+      <c r="A148" t="s">
+        <v>506</v>
+      </c>
+      <c r="B148" t="s">
+        <v>507</v>
+      </c>
+      <c r="C148" t="s">
+        <v>508</v>
+      </c>
+      <c r="I148" t="s">
+        <v>432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added obj000105 and pics to source files
</commit_message>
<xml_diff>
--- a/externals/Eve_web_catalog.xlsx
+++ b/externals/Eve_web_catalog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="60" windowWidth="24040" windowHeight="11420" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="540" yWindow="60" windowWidth="24040" windowHeight="11420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="515">
   <si>
     <t>000025-01</t>
   </si>
@@ -1549,6 +1549,24 @@
   </si>
   <si>
     <t>S-40-0048</t>
+  </si>
+  <si>
+    <t>pic000208</t>
+  </si>
+  <si>
+    <t>alb000105</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000208.textile</t>
+  </si>
+  <si>
+    <t>S-1-0005</t>
+  </si>
+  <si>
+    <t>textile arts</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000105-01.textile</t>
   </si>
 </sst>
 </file>
@@ -2105,8 +2123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I73"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="C29" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3178,6 +3196,27 @@
       <c r="A44" t="s">
         <v>438</v>
       </c>
+      <c r="B44" t="s">
+        <v>514</v>
+      </c>
+      <c r="C44" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" t="s">
+        <v>421</v>
+      </c>
+      <c r="F44" t="s">
+        <v>420</v>
+      </c>
+      <c r="G44" t="s">
+        <v>509</v>
+      </c>
+      <c r="H44" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
@@ -3392,9 +3431,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J148"/>
+  <dimension ref="A2:J149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="A137" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="I149" sqref="I149"/>
     </sheetView>
   </sheetViews>
@@ -5077,6 +5116,20 @@
         <v>432</v>
       </c>
     </row>
+    <row r="149" spans="1:9">
+      <c r="A149" t="s">
+        <v>509</v>
+      </c>
+      <c r="B149" t="s">
+        <v>511</v>
+      </c>
+      <c r="C149" t="s">
+        <v>512</v>
+      </c>
+      <c r="I149" t="s">
+        <v>510</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5091,10 +5144,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:B11"/>
+  <dimension ref="B4:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5127,6 +5180,11 @@
     <row r="11" spans="2:2">
       <c r="B11" t="s">
         <v>491</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" t="s">
+        <v>510</v>
       </c>
     </row>
   </sheetData>
@@ -5143,10 +5201,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D3"/>
+  <dimension ref="B2:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5167,6 +5225,11 @@
         <v>492</v>
       </c>
     </row>
+    <row r="4" spans="2:4">
+      <c r="B4" t="s">
+        <v>513</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
added OBJs 106, 107, 108 and associated source files
</commit_message>
<xml_diff>
--- a/externals/Eve_web_catalog.xlsx
+++ b/externals/Eve_web_catalog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="60" windowWidth="24040" windowHeight="11420" tabRatio="500"/>
+    <workbookView xWindow="2120" yWindow="1080" windowWidth="27460" windowHeight="7480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="530">
   <si>
     <t>000025-01</t>
   </si>
@@ -1563,10 +1563,55 @@
     <t>S-1-0005</t>
   </si>
   <si>
-    <t>textile arts</t>
-  </si>
-  <si>
     <t>2015-08-09-obj000105-01.textile</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000106-01.textile</t>
+  </si>
+  <si>
+    <t>pic000209</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000209.textile</t>
+  </si>
+  <si>
+    <t>S-3-0031.jpg</t>
+  </si>
+  <si>
+    <t>alb000106</t>
+  </si>
+  <si>
+    <t>textile art</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000107-01.textile</t>
+  </si>
+  <si>
+    <t>pic000210</t>
+  </si>
+  <si>
+    <t>alb000107</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000210.textile</t>
+  </si>
+  <si>
+    <t>S-14-0021.jpg</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000108-01.textile</t>
+  </si>
+  <si>
+    <t>pic000211</t>
+  </si>
+  <si>
+    <t>alb000108</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000211.textile</t>
+  </si>
+  <si>
+    <t>S-15-0024.jpg</t>
   </si>
 </sst>
 </file>
@@ -1646,8 +1691,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="67">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1725,7 +1786,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="67">
+  <cellStyles count="83">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1759,6 +1820,14 @@
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1792,6 +1861,14 @@
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2123,8 +2200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C29" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView topLeftCell="A42" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3197,7 +3274,7 @@
         <v>438</v>
       </c>
       <c r="B44" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C44" t="s">
         <v>3</v>
@@ -3222,15 +3299,78 @@
       <c r="A45" t="s">
         <v>439</v>
       </c>
+      <c r="B45" t="s">
+        <v>514</v>
+      </c>
+      <c r="C45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" t="s">
+        <v>421</v>
+      </c>
+      <c r="F45" t="s">
+        <v>420</v>
+      </c>
+      <c r="G45" t="s">
+        <v>515</v>
+      </c>
+      <c r="H45" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>440</v>
       </c>
+      <c r="B46" t="s">
+        <v>520</v>
+      </c>
+      <c r="C46" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" t="s">
+        <v>421</v>
+      </c>
+      <c r="F46" t="s">
+        <v>420</v>
+      </c>
+      <c r="G46" t="s">
+        <v>521</v>
+      </c>
+      <c r="H46" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>441</v>
+      </c>
+      <c r="B47" t="s">
+        <v>525</v>
+      </c>
+      <c r="C47" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" t="s">
+        <v>421</v>
+      </c>
+      <c r="F47" t="s">
+        <v>420</v>
+      </c>
+      <c r="G47" t="s">
+        <v>526</v>
+      </c>
+      <c r="H47" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -3431,10 +3571,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J149"/>
+  <dimension ref="A2:J152"/>
   <sheetViews>
-    <sheetView topLeftCell="A137" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I149" sqref="I149"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C153" sqref="C153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5130,6 +5270,48 @@
         <v>510</v>
       </c>
     </row>
+    <row r="150" spans="1:9">
+      <c r="A150" t="s">
+        <v>515</v>
+      </c>
+      <c r="B150" t="s">
+        <v>516</v>
+      </c>
+      <c r="C150" t="s">
+        <v>517</v>
+      </c>
+      <c r="I150" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9">
+      <c r="A151" t="s">
+        <v>521</v>
+      </c>
+      <c r="B151" t="s">
+        <v>523</v>
+      </c>
+      <c r="C151" t="s">
+        <v>524</v>
+      </c>
+      <c r="I151" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9">
+      <c r="A152" t="s">
+        <v>526</v>
+      </c>
+      <c r="B152" t="s">
+        <v>528</v>
+      </c>
+      <c r="C152" t="s">
+        <v>529</v>
+      </c>
+      <c r="I152" t="s">
+        <v>527</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5144,10 +5326,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:B12"/>
+  <dimension ref="B4:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5185,6 +5367,21 @@
     <row r="12" spans="2:2">
       <c r="B12" t="s">
         <v>510</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2">
+      <c r="B15" t="s">
+        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -5204,7 +5401,7 @@
   <dimension ref="B2:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5227,7 +5424,7 @@
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
-        <v>513</v>
+        <v>519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added OJB 109 and assoc. source files
</commit_message>
<xml_diff>
--- a/externals/Eve_web_catalog.xlsx
+++ b/externals/Eve_web_catalog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="1080" windowWidth="27460" windowHeight="7480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="100" yWindow="200" windowWidth="27840" windowHeight="10780" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="534">
   <si>
     <t>000025-01</t>
   </si>
@@ -1612,6 +1612,18 @@
   </si>
   <si>
     <t>S-15-0024.jpg</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000109-01.textile</t>
+  </si>
+  <si>
+    <t>pic000212</t>
+  </si>
+  <si>
+    <t>alb000109</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000212.textile</t>
   </si>
 </sst>
 </file>
@@ -1691,8 +1703,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="83">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1786,7 +1806,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="83">
+  <cellStyles count="91">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1828,6 +1848,10 @@
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1869,6 +1893,10 @@
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2200,7 +2228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I73"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="A39" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
@@ -3377,6 +3405,27 @@
       <c r="A48" t="s">
         <v>442</v>
       </c>
+      <c r="B48" t="s">
+        <v>530</v>
+      </c>
+      <c r="C48" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" t="s">
+        <v>421</v>
+      </c>
+      <c r="F48" t="s">
+        <v>420</v>
+      </c>
+      <c r="G48" t="s">
+        <v>531</v>
+      </c>
+      <c r="H48" t="s">
+        <v>532</v>
+      </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
@@ -3571,7 +3620,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J152"/>
+  <dimension ref="A2:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A148" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C153" sqref="C153"/>
@@ -5312,6 +5361,20 @@
         <v>527</v>
       </c>
     </row>
+    <row r="153" spans="1:9">
+      <c r="A153" t="s">
+        <v>531</v>
+      </c>
+      <c r="B153" t="s">
+        <v>533</v>
+      </c>
+      <c r="C153" t="s">
+        <v>529</v>
+      </c>
+      <c r="I153" t="s">
+        <v>532</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5326,10 +5389,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:B15"/>
+  <dimension ref="B4:B16"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5382,6 +5445,11 @@
     <row r="15" spans="2:2">
       <c r="B15" t="s">
         <v>527</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2">
+      <c r="B16" t="s">
+        <v>532</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added source files for OBJs110-116
</commit_message>
<xml_diff>
--- a/externals/Eve_web_catalog.xlsx
+++ b/externals/Eve_web_catalog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="200" windowWidth="27840" windowHeight="10780" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1800" yWindow="7320" windowWidth="25780" windowHeight="8760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="569">
   <si>
     <t>000025-01</t>
   </si>
@@ -1624,13 +1624,118 @@
   </si>
   <si>
     <t>2015-08-09-pic000212.textile</t>
+  </si>
+  <si>
+    <t>pic000213</t>
+  </si>
+  <si>
+    <t>S-18-0036.jpg</t>
+  </si>
+  <si>
+    <t>alb000110</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000213.textile</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000110-01.textile</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000111-01.textile</t>
+  </si>
+  <si>
+    <t>pic000214</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000214.textile</t>
+  </si>
+  <si>
+    <t>S-19-0010.jpg</t>
+  </si>
+  <si>
+    <t>alb000111</t>
+  </si>
+  <si>
+    <t>alb000112</t>
+  </si>
+  <si>
+    <t>S-20-0014.jpg</t>
+  </si>
+  <si>
+    <t>pic000215</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000215.textile</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000112-01.textile</t>
+  </si>
+  <si>
+    <t>alb000113</t>
+  </si>
+  <si>
+    <t>S-21-0027.jpg</t>
+  </si>
+  <si>
+    <t>pic000216</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000216.textile</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000113-01.textile</t>
+  </si>
+  <si>
+    <t>alb000114</t>
+  </si>
+  <si>
+    <t>pic000217</t>
+  </si>
+  <si>
+    <t>S-29-0001</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000217.textile</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000114-01.textile</t>
+  </si>
+  <si>
+    <t>S-30-1</t>
+  </si>
+  <si>
+    <t>pic000218</t>
+  </si>
+  <si>
+    <t>alb000115</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000218.textile</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000115-01.textile</t>
+  </si>
+  <si>
+    <t>pic000219</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000219.textile</t>
+  </si>
+  <si>
+    <t>S-31-0012</t>
+  </si>
+  <si>
+    <t>alb000116</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000116-01.textile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1685,6 +1790,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1703,7 +1813,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="91">
+  <cellStyleXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1795,8 +1905,94 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1805,8 +2001,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="91">
+  <cellStyles count="177">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1852,6 +2049,49 @@
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1897,6 +2137,49 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2228,8 +2511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I73"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55:F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3427,82 +3710,229 @@
         <v>532</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="B49" t="s">
+        <v>538</v>
+      </c>
+      <c r="C49" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" t="s">
+        <v>421</v>
+      </c>
+      <c r="F49" t="s">
+        <v>420</v>
+      </c>
+      <c r="G49" t="s">
+        <v>534</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="B50" t="s">
+        <v>539</v>
+      </c>
+      <c r="C50" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" t="s">
+        <v>421</v>
+      </c>
+      <c r="F50" t="s">
+        <v>420</v>
+      </c>
+      <c r="G50" t="s">
+        <v>540</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
+      <c r="B51" t="s">
+        <v>548</v>
+      </c>
+      <c r="C51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" t="s">
+        <v>421</v>
+      </c>
+      <c r="F51" t="s">
+        <v>420</v>
+      </c>
+      <c r="G51" t="s">
+        <v>546</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="53" spans="1:1">
+      <c r="B52" t="s">
+        <v>553</v>
+      </c>
+      <c r="C52" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52" t="s">
+        <v>421</v>
+      </c>
+      <c r="F52" t="s">
+        <v>420</v>
+      </c>
+      <c r="G52" t="s">
+        <v>551</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="54" spans="1:1">
+      <c r="B53" t="s">
+        <v>558</v>
+      </c>
+      <c r="C53" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" t="s">
+        <v>4</v>
+      </c>
+      <c r="E53" t="s">
+        <v>421</v>
+      </c>
+      <c r="F53" t="s">
+        <v>420</v>
+      </c>
+      <c r="G53" t="s">
+        <v>555</v>
+      </c>
+      <c r="H53" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="55" spans="1:1">
+      <c r="B54" t="s">
+        <v>563</v>
+      </c>
+      <c r="C54" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" t="s">
+        <v>421</v>
+      </c>
+      <c r="F54" t="s">
+        <v>420</v>
+      </c>
+      <c r="G54" t="s">
+        <v>560</v>
+      </c>
+      <c r="H54" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="B55" t="s">
+        <v>568</v>
+      </c>
+      <c r="C55" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55" t="s">
+        <v>4</v>
+      </c>
+      <c r="E55" t="s">
+        <v>421</v>
+      </c>
+      <c r="F55" t="s">
+        <v>420</v>
+      </c>
+      <c r="G55" t="s">
+        <v>564</v>
+      </c>
+      <c r="H55" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
         <v>458</v>
       </c>
@@ -3620,10 +4050,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J153"/>
+  <dimension ref="A2:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C153" sqref="C153"/>
+    <sheetView topLeftCell="A152" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I160" sqref="I160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5375,6 +5805,104 @@
         <v>532</v>
       </c>
     </row>
+    <row r="154" spans="1:9">
+      <c r="A154" t="s">
+        <v>534</v>
+      </c>
+      <c r="B154" t="s">
+        <v>537</v>
+      </c>
+      <c r="C154" t="s">
+        <v>535</v>
+      </c>
+      <c r="I154" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9">
+      <c r="A155" t="s">
+        <v>540</v>
+      </c>
+      <c r="B155" t="s">
+        <v>541</v>
+      </c>
+      <c r="C155" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="I155" s="3" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9">
+      <c r="A156" t="s">
+        <v>546</v>
+      </c>
+      <c r="B156" t="s">
+        <v>547</v>
+      </c>
+      <c r="C156" s="6" t="s">
+        <v>545</v>
+      </c>
+      <c r="I156" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9">
+      <c r="A157" t="s">
+        <v>551</v>
+      </c>
+      <c r="B157" t="s">
+        <v>552</v>
+      </c>
+      <c r="C157" t="s">
+        <v>550</v>
+      </c>
+      <c r="I157" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9">
+      <c r="A158" t="s">
+        <v>555</v>
+      </c>
+      <c r="B158" t="s">
+        <v>557</v>
+      </c>
+      <c r="C158" t="s">
+        <v>556</v>
+      </c>
+      <c r="I158" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9">
+      <c r="A159" t="s">
+        <v>560</v>
+      </c>
+      <c r="B159" t="s">
+        <v>562</v>
+      </c>
+      <c r="C159" t="s">
+        <v>559</v>
+      </c>
+      <c r="I159" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9">
+      <c r="A160" t="s">
+        <v>564</v>
+      </c>
+      <c r="B160" t="s">
+        <v>565</v>
+      </c>
+      <c r="C160" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="I160" t="s">
+        <v>567</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5389,10 +5917,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:B16"/>
+  <dimension ref="B4:B23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5450,6 +5978,41 @@
     <row r="16" spans="2:2">
       <c r="B16" t="s">
         <v>532</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" t="s">
+        <v>567</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added sourcefiles for OBJs 118, 119, 120, 121
</commit_message>
<xml_diff>
--- a/externals/Eve_web_catalog.xlsx
+++ b/externals/Eve_web_catalog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="7320" windowWidth="25780" windowHeight="8760" tabRatio="500"/>
+    <workbookView xWindow="380" yWindow="4480" windowWidth="25780" windowHeight="8740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="584">
   <si>
     <t>000025-01</t>
   </si>
@@ -1729,6 +1729,51 @@
   </si>
   <si>
     <t>2015-08-09-obj000116-01.textile</t>
+  </si>
+  <si>
+    <t>pic000220</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000220.textile</t>
+  </si>
+  <si>
+    <t>alb000117</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000117-01.textile</t>
+  </si>
+  <si>
+    <t>pic000221</t>
+  </si>
+  <si>
+    <t>S-33-0021</t>
+  </si>
+  <si>
+    <t>S-32-0018</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000221.textile</t>
+  </si>
+  <si>
+    <t>alb000118</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000118-01.textile</t>
+  </si>
+  <si>
+    <t>S-34-0065</t>
+  </si>
+  <si>
+    <t>pic000222</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000222.textile</t>
+  </si>
+  <si>
+    <t>alb000119</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000119-01.textile</t>
   </si>
 </sst>
 </file>
@@ -1813,8 +1858,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="177">
+  <cellStyleXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2003,7 +2066,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="177">
+  <cellStyles count="195">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2092,6 +2155,15 @@
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2180,6 +2252,15 @@
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2511,8 +2592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55:F55"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3896,15 +3977,78 @@
       <c r="A56" t="s">
         <v>450</v>
       </c>
+      <c r="B56" t="s">
+        <v>572</v>
+      </c>
+      <c r="C56" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" t="s">
+        <v>421</v>
+      </c>
+      <c r="F56" t="s">
+        <v>420</v>
+      </c>
+      <c r="G56" t="s">
+        <v>569</v>
+      </c>
+      <c r="H56" t="s">
+        <v>571</v>
+      </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>451</v>
       </c>
+      <c r="B57" t="s">
+        <v>578</v>
+      </c>
+      <c r="C57" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" t="s">
+        <v>421</v>
+      </c>
+      <c r="F57" t="s">
+        <v>420</v>
+      </c>
+      <c r="G57" t="s">
+        <v>573</v>
+      </c>
+      <c r="H57" t="s">
+        <v>577</v>
+      </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>452</v>
+      </c>
+      <c r="B58" t="s">
+        <v>583</v>
+      </c>
+      <c r="C58" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" t="s">
+        <v>4</v>
+      </c>
+      <c r="E58" t="s">
+        <v>421</v>
+      </c>
+      <c r="F58" t="s">
+        <v>420</v>
+      </c>
+      <c r="G58" t="s">
+        <v>580</v>
+      </c>
+      <c r="H58" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -4050,10 +4194,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J160"/>
+  <dimension ref="A2:J163"/>
   <sheetViews>
-    <sheetView topLeftCell="A152" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I160" sqref="I160"/>
+    <sheetView topLeftCell="A154" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C163" sqref="C163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5903,6 +6047,48 @@
         <v>567</v>
       </c>
     </row>
+    <row r="161" spans="1:9">
+      <c r="A161" t="s">
+        <v>569</v>
+      </c>
+      <c r="B161" t="s">
+        <v>570</v>
+      </c>
+      <c r="C161" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="I161" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9">
+      <c r="A162" t="s">
+        <v>573</v>
+      </c>
+      <c r="B162" t="s">
+        <v>576</v>
+      </c>
+      <c r="C162" s="6" t="s">
+        <v>575</v>
+      </c>
+      <c r="I162" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9">
+      <c r="A163" t="s">
+        <v>580</v>
+      </c>
+      <c r="B163" t="s">
+        <v>581</v>
+      </c>
+      <c r="C163" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="I163" t="s">
+        <v>582</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5917,10 +6103,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:B23"/>
+  <dimension ref="B4:B26"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6013,6 +6199,21 @@
     <row r="23" spans="2:2">
       <c r="B23" t="s">
         <v>567</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" t="s">
+        <v>582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added sourcefiles for OBJs 122, 123, 124, 125
</commit_message>
<xml_diff>
--- a/externals/Eve_web_catalog.xlsx
+++ b/externals/Eve_web_catalog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="4480" windowWidth="25780" windowHeight="8740" tabRatio="500"/>
+    <workbookView xWindow="1560" yWindow="8580" windowWidth="25780" windowHeight="8760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="615">
   <si>
     <t>000025-01</t>
   </si>
@@ -1774,13 +1774,106 @@
   </si>
   <si>
     <t>2015-08-09-obj000119-01.textile</t>
+  </si>
+  <si>
+    <t>pic000223</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000223.textile</t>
+  </si>
+  <si>
+    <t>S-35-0072</t>
+  </si>
+  <si>
+    <t>alb000120</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000120-01.textile</t>
+  </si>
+  <si>
+    <t>pic000224</t>
+  </si>
+  <si>
+    <t>S-36-0075</t>
+  </si>
+  <si>
+    <t>alb000121</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000224.textile</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000121-01.textile</t>
+  </si>
+  <si>
+    <t>S-37-0082</t>
+  </si>
+  <si>
+    <t>pic000225</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000225.textile</t>
+  </si>
+  <si>
+    <t>alb000122</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000122-01.textile</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000226.textile</t>
+  </si>
+  <si>
+    <t>pic000226</t>
+  </si>
+  <si>
+    <t>S-38-0085</t>
+  </si>
+  <si>
+    <t>alb000123</t>
+  </si>
+  <si>
+    <t>pic000227</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000227.textile</t>
+  </si>
+  <si>
+    <t>S-39-0089</t>
+  </si>
+  <si>
+    <t>alb000124</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000123-01.textile</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000124-01.textile</t>
+  </si>
+  <si>
+    <t>obj000124-01</t>
+  </si>
+  <si>
+    <t>pic000228</t>
+  </si>
+  <si>
+    <t>S-39-0093</t>
+  </si>
+  <si>
+    <t>alb000125</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000228.textile</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000125-01.textile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1840,6 +1933,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1858,7 +1957,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="195">
+  <cellStyleXfs count="231">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2054,8 +2153,44 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2065,8 +2200,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="195">
+  <cellStyles count="231">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2164,6 +2300,24 @@
     <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2261,6 +2415,24 @@
     <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2590,10 +2762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I73"/>
+  <dimension ref="A2:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64:F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4055,91 +4227,199 @@
       <c r="A59" t="s">
         <v>453</v>
       </c>
+      <c r="B59" t="s">
+        <v>588</v>
+      </c>
+      <c r="C59" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" t="s">
+        <v>4</v>
+      </c>
+      <c r="E59" t="s">
+        <v>421</v>
+      </c>
+      <c r="F59" t="s">
+        <v>420</v>
+      </c>
+      <c r="G59" t="s">
+        <v>584</v>
+      </c>
+      <c r="H59" t="s">
+        <v>587</v>
+      </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>454</v>
       </c>
+      <c r="B60" t="s">
+        <v>593</v>
+      </c>
+      <c r="C60" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" t="s">
+        <v>421</v>
+      </c>
+      <c r="F60" t="s">
+        <v>420</v>
+      </c>
+      <c r="G60" t="s">
+        <v>589</v>
+      </c>
+      <c r="H60" t="s">
+        <v>591</v>
+      </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>455</v>
       </c>
+      <c r="B61" t="s">
+        <v>598</v>
+      </c>
+      <c r="C61" t="s">
+        <v>3</v>
+      </c>
+      <c r="D61" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" t="s">
+        <v>421</v>
+      </c>
+      <c r="F61" t="s">
+        <v>420</v>
+      </c>
+      <c r="G61" t="s">
+        <v>595</v>
+      </c>
+      <c r="H61" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
         <v>456</v>
       </c>
+      <c r="B62" t="s">
+        <v>607</v>
+      </c>
+      <c r="C62" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" t="s">
+        <v>421</v>
+      </c>
+      <c r="F62" t="s">
+        <v>420</v>
+      </c>
+      <c r="G62" t="s">
+        <v>600</v>
+      </c>
+      <c r="H62" t="s">
+        <v>602</v>
+      </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
-        <v>457</v>
+        <v>609</v>
+      </c>
+      <c r="B63" t="s">
+        <v>608</v>
+      </c>
+      <c r="C63" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" t="s">
+        <v>421</v>
+      </c>
+      <c r="F63" t="s">
+        <v>420</v>
+      </c>
+      <c r="G63" t="s">
+        <v>603</v>
+      </c>
+      <c r="H63" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>458</v>
+        <v>457</v>
+      </c>
+      <c r="B64" t="s">
+        <v>614</v>
+      </c>
+      <c r="C64" t="s">
+        <v>3</v>
+      </c>
+      <c r="D64" t="s">
+        <v>4</v>
+      </c>
+      <c r="E64" t="s">
+        <v>421</v>
+      </c>
+      <c r="F64" t="s">
+        <v>420</v>
+      </c>
+      <c r="G64" t="s">
+        <v>610</v>
+      </c>
+      <c r="H64" t="s">
+        <v>612</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>463</v>
-      </c>
-      <c r="B71" t="s">
-        <v>469</v>
-      </c>
-      <c r="C71" t="s">
-        <v>3</v>
-      </c>
-      <c r="D71" t="s">
-        <v>470</v>
-      </c>
-      <c r="E71" t="s">
-        <v>471</v>
-      </c>
-      <c r="G71" t="s">
-        <v>473</v>
-      </c>
-      <c r="H71" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>475</v>
+        <v>463</v>
       </c>
       <c r="B72" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="C72" t="s">
         <v>3</v>
@@ -4148,21 +4428,21 @@
         <v>470</v>
       </c>
       <c r="E72" t="s">
-        <v>477</v>
-      </c>
-      <c r="F72" t="s">
-        <v>97</v>
+        <v>471</v>
       </c>
       <c r="G72" t="s">
-        <v>474</v>
+        <v>473</v>
+      </c>
+      <c r="H72" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B73" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="C73" t="s">
         <v>3</v>
@@ -4171,12 +4451,35 @@
         <v>470</v>
       </c>
       <c r="E73" t="s">
+        <v>477</v>
+      </c>
+      <c r="F73" t="s">
+        <v>97</v>
+      </c>
+      <c r="G73" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" t="s">
+        <v>478</v>
+      </c>
+      <c r="B74" t="s">
+        <v>482</v>
+      </c>
+      <c r="C74" t="s">
+        <v>3</v>
+      </c>
+      <c r="D74" t="s">
+        <v>470</v>
+      </c>
+      <c r="E74" t="s">
         <v>480</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F74" t="s">
         <v>481</v>
       </c>
-      <c r="G73" t="s">
+      <c r="G74" t="s">
         <v>479</v>
       </c>
     </row>
@@ -4194,10 +4497,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J163"/>
+  <dimension ref="A2:J169"/>
   <sheetViews>
-    <sheetView topLeftCell="A154" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C163" sqref="C163"/>
+    <sheetView topLeftCell="A161" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B170" sqref="B170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6089,6 +6392,90 @@
         <v>582</v>
       </c>
     </row>
+    <row r="164" spans="1:9">
+      <c r="A164" t="s">
+        <v>584</v>
+      </c>
+      <c r="B164" t="s">
+        <v>585</v>
+      </c>
+      <c r="C164" s="7" t="s">
+        <v>586</v>
+      </c>
+      <c r="I164" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9">
+      <c r="A165" t="s">
+        <v>589</v>
+      </c>
+      <c r="B165" t="s">
+        <v>592</v>
+      </c>
+      <c r="C165" s="6" t="s">
+        <v>590</v>
+      </c>
+      <c r="I165" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9">
+      <c r="A166" t="s">
+        <v>595</v>
+      </c>
+      <c r="B166" t="s">
+        <v>596</v>
+      </c>
+      <c r="C166" s="6" t="s">
+        <v>594</v>
+      </c>
+      <c r="I166" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9">
+      <c r="A167" t="s">
+        <v>600</v>
+      </c>
+      <c r="B167" t="s">
+        <v>599</v>
+      </c>
+      <c r="C167" t="s">
+        <v>601</v>
+      </c>
+      <c r="I167" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9">
+      <c r="A168" t="s">
+        <v>603</v>
+      </c>
+      <c r="B168" t="s">
+        <v>604</v>
+      </c>
+      <c r="C168" t="s">
+        <v>605</v>
+      </c>
+      <c r="I168" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9">
+      <c r="A169" t="s">
+        <v>610</v>
+      </c>
+      <c r="B169" t="s">
+        <v>613</v>
+      </c>
+      <c r="C169" t="s">
+        <v>611</v>
+      </c>
+      <c r="I169" t="s">
+        <v>612</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6103,10 +6490,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:B26"/>
+  <dimension ref="B4:B32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6214,6 +6601,36 @@
     <row r="26" spans="2:2">
       <c r="B26" t="s">
         <v>582</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" t="s">
+        <v>612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made source files for OBJs 126-130, with draft Textile files for 129 and 130
</commit_message>
<xml_diff>
--- a/externals/Eve_web_catalog.xlsx
+++ b/externals/Eve_web_catalog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="8580" windowWidth="25780" windowHeight="8760" tabRatio="500"/>
+    <workbookView xWindow="720" yWindow="10020" windowWidth="25780" windowHeight="8760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="625">
   <si>
     <t>000025-01</t>
   </si>
@@ -1867,6 +1867,36 @@
   </si>
   <si>
     <t>2015-08-09-obj000125-01.textile</t>
+  </si>
+  <si>
+    <t>pic000229</t>
+  </si>
+  <si>
+    <t>S-12-0012</t>
+  </si>
+  <si>
+    <t>alb000126</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000229.textile</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000126-01.textile</t>
+  </si>
+  <si>
+    <t>Collage/photo</t>
+  </si>
+  <si>
+    <t>Days of 1988 (summer)</t>
+  </si>
+  <si>
+    <t>pic000230</t>
+  </si>
+  <si>
+    <t>S-13-0006</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000230.textile</t>
   </si>
 </sst>
 </file>
@@ -1957,8 +1987,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="231">
+  <cellStyleXfs count="249">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2202,7 +2250,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="231">
+  <cellStyles count="249">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2318,6 +2366,15 @@
     <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2433,6 +2490,15 @@
     <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2764,8 +2830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64:F64"/>
+    <sheetView topLeftCell="A57" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4383,6 +4449,27 @@
       <c r="A65" t="s">
         <v>458</v>
       </c>
+      <c r="B65" t="s">
+        <v>619</v>
+      </c>
+      <c r="C65" t="s">
+        <v>3</v>
+      </c>
+      <c r="D65" t="s">
+        <v>4</v>
+      </c>
+      <c r="E65" t="s">
+        <v>620</v>
+      </c>
+      <c r="F65" t="s">
+        <v>621</v>
+      </c>
+      <c r="G65" t="s">
+        <v>615</v>
+      </c>
+      <c r="H65" t="s">
+        <v>617</v>
+      </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
@@ -4497,10 +4584,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J169"/>
+  <dimension ref="A2:J171"/>
   <sheetViews>
-    <sheetView topLeftCell="A161" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B170" sqref="B170"/>
+    <sheetView tabSelected="1" topLeftCell="A161" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B171" sqref="B171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6476,6 +6563,31 @@
         <v>612</v>
       </c>
     </row>
+    <row r="170" spans="1:9">
+      <c r="A170" t="s">
+        <v>615</v>
+      </c>
+      <c r="B170" t="s">
+        <v>618</v>
+      </c>
+      <c r="C170" t="s">
+        <v>616</v>
+      </c>
+      <c r="I170" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9">
+      <c r="A171" t="s">
+        <v>622</v>
+      </c>
+      <c r="B171" t="s">
+        <v>624</v>
+      </c>
+      <c r="C171" t="s">
+        <v>623</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6490,10 +6602,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:B32"/>
+  <dimension ref="B4:B33"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6631,6 +6743,11 @@
     <row r="32" spans="2:2">
       <c r="B32" t="s">
         <v>612</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change LO files to remove descriptions from category lists and add to individual artworks pages. Corrections to Obj127, 128, 129 and 130 Textile files
</commit_message>
<xml_diff>
--- a/externals/Eve_web_catalog.xlsx
+++ b/externals/Eve_web_catalog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="10020" windowWidth="25780" windowHeight="8760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="6020" yWindow="6860" windowWidth="25780" windowHeight="8840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="645">
   <si>
     <t>000025-01</t>
   </si>
@@ -1897,6 +1897,66 @@
   </si>
   <si>
     <t>2015-08-09-pic000230.textile</t>
+  </si>
+  <si>
+    <t>alb000127</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000127-01.textile</t>
+  </si>
+  <si>
+    <t>pic000231</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000231.textile</t>
+  </si>
+  <si>
+    <t>S 23-0018</t>
+  </si>
+  <si>
+    <t>alb000128</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Eternity’s White Flag - Before - / And God- at every Gate-</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000128-01.textile</t>
+  </si>
+  <si>
+    <t>Jacket Night at the ID450 Collective</t>
+  </si>
+  <si>
+    <t>pic000232</t>
+  </si>
+  <si>
+    <t>S 28-0007</t>
+  </si>
+  <si>
+    <t>alb000129</t>
+  </si>
+  <si>
+    <t>Terrible Scrabble</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000129-01.textile</t>
+  </si>
+  <si>
+    <t>2015-08-09-pic000233.textile</t>
+  </si>
+  <si>
+    <t>alb000130</t>
+  </si>
+  <si>
+    <t>S 43-0034</t>
+  </si>
+  <si>
+    <t>Listening to Dionne (1)</t>
+  </si>
+  <si>
+    <t>2015-08-09-obj000130-01.textile</t>
+  </si>
+  <si>
+    <t>pic000233</t>
   </si>
 </sst>
 </file>
@@ -1987,8 +2047,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="249">
+  <cellStyleXfs count="275">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2250,7 +2336,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="249">
+  <cellStyles count="275">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2375,6 +2461,19 @@
     <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2499,6 +2598,19 @@
     <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2830,8 +2942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I74"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4475,20 +4587,104 @@
       <c r="A66" t="s">
         <v>459</v>
       </c>
+      <c r="B66" t="s">
+        <v>626</v>
+      </c>
+      <c r="C66" t="s">
+        <v>3</v>
+      </c>
+      <c r="D66" t="s">
+        <v>4</v>
+      </c>
+      <c r="E66" t="s">
+        <v>620</v>
+      </c>
+      <c r="F66" t="s">
+        <v>631</v>
+      </c>
+      <c r="G66" t="s">
+        <v>622</v>
+      </c>
+      <c r="H66" t="s">
+        <v>625</v>
+      </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
         <v>460</v>
       </c>
+      <c r="B67" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="H67" t="s">
+        <v>630</v>
+      </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
         <v>461</v>
       </c>
+      <c r="B68" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="F68" t="s">
+        <v>637</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="H68" t="s">
+        <v>636</v>
+      </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>462</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="F69" t="s">
+        <v>642</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="H69" t="s">
+        <v>640</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -4584,10 +4780,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J171"/>
+  <dimension ref="A2:J174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B171" sqref="B171"/>
+    <sheetView topLeftCell="A165" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A175" sqref="A175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6587,6 +6783,61 @@
       <c r="C171" t="s">
         <v>623</v>
       </c>
+      <c r="I171" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9">
+      <c r="A172" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="D172" s="3"/>
+      <c r="E172" s="3"/>
+      <c r="F172" s="3"/>
+      <c r="G172" s="3"/>
+      <c r="H172" s="3"/>
+      <c r="I172" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9">
+      <c r="A173" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="D173" s="3"/>
+      <c r="E173" s="3"/>
+      <c r="F173" s="3"/>
+      <c r="G173" s="3"/>
+      <c r="H173" s="3"/>
+      <c r="I173" s="3" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9">
+      <c r="A174" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="B174" t="s">
+        <v>639</v>
+      </c>
+      <c r="C174" t="s">
+        <v>641</v>
+      </c>
+      <c r="I174" s="3" t="s">
+        <v>640</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -6602,10 +6853,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:B33"/>
+  <dimension ref="B4:B37"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6748,6 +6999,26 @@
     <row r="33" spans="2:2">
       <c r="B33" t="s">
         <v>617</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" t="s">
+        <v>640</v>
       </c>
     </row>
   </sheetData>

</xml_diff>